<commit_message>
unit test for investment_account.py
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Updated Assignments ISD\assignment_02\given_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c3d6174ceab06f3/Desktop/rrc_polytech/courses_term2/intermediate_software_development/project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{9D6AEFC8-F3D7-467B-9A12-00596A3BA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E575987A-26B7-4397-B940-2D91F59DC372}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="25185" windowHeight="13845" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView minimized="1" xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="8880" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{3AFD6792-4858-4432-8D1A-2CB895E262E1}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{3AFD6792-4858-4432-8D1A-2CB895E262E1}">
       <text>
         <r>
           <rPr>
@@ -80,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{E95CB908-567C-490A-A2E2-01BADA61CAE4}">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{E95CB908-567C-490A-A2E2-01BADA61CAE4}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{8F1D4BE8-86F7-4F2B-9CF2-29A2362B0A96}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{8F1D4BE8-86F7-4F2B-9CF2-29A2362B0A96}">
       <text>
         <r>
           <rPr>
@@ -106,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{81A699C9-D13C-46A8-BDED-9E9372CFC271}">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{81A699C9-D13C-46A8-BDED-9E9372CFC271}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{A9B43634-DF5E-47A8-B694-39F3725B8514}">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{A9B43634-DF5E-47A8-B694-39F3725B8514}">
       <text>
         <r>
           <rPr>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{CACC1002-2768-4B77-8035-B63564EBC973}">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{CACC1002-2768-4B77-8035-B63564EBC973}">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -246,6 +246,18 @@
   </si>
   <si>
     <t>date created exactly 10 years ago.</t>
+  </si>
+  <si>
+    <t>Jashanpreet Kaur Jattana</t>
+  </si>
+  <si>
+    <t>Valid account number, balance, and date created</t>
+  </si>
+  <si>
+    <t>Invalid management fee type</t>
+  </si>
+  <si>
+    <t>Date created more than 10 years ago</t>
   </si>
 </sst>
 </file>
@@ -820,7 +832,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="B6:G32" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7B0B8C9F-A34D-46F3-9066-19FDAF76B033}" name="Table1" displayName="Table1" ref="C6:H32" totalsRowShown="0" headerRowDxfId="6">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B4BB882C-2019-4F87-8900-426FA9A11FFB}" name="Test Case ID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{1904C92F-9639-4229-AA4E-4C4DEAF21EEE}" name="Method being Tested" dataDxfId="4"/>
@@ -1150,24 +1162,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="27.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="49.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1179,14 +1191,16 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1195,318 +1209,324 @@
       </c>
       <c r="D4" s="20"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="G6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11">
+    <row r="7" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="11">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3">
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11">
+      <c r="F8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
+      <c r="F9" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11">
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="11">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11">
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="11">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:8" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="3">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="11">
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="11">
         <v>7</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11">
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="11">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
       <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11">
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="11">
         <v>9</v>
       </c>
-      <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="2:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="3">
         <v>10</v>
       </c>
-      <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="11">
         <v>11</v>
       </c>
-      <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="11">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="11">
         <v>12</v>
       </c>
-      <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11">
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="3:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="11">
         <v>13</v>
       </c>
-      <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="3">
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="3">
         <v>14</v>
       </c>
-      <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11">
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="11">
         <v>15</v>
       </c>
-      <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11">
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="11">
         <v>16</v>
       </c>
-      <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="3:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="11">
         <v>17</v>
       </c>
-      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="3">
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="3">
         <v>18</v>
       </c>
-      <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="11">
         <v>19</v>
       </c>
-      <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11">
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="11">
         <v>20</v>
       </c>
-      <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="3:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="11">
         <v>21</v>
       </c>
-      <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="3">
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="3">
         <v>22</v>
       </c>
-      <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11">
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="11">
         <v>23</v>
       </c>
-      <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-    </row>
-    <row r="30" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="11">
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="11">
         <v>24</v>
       </c>
-      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11">
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="3:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="11">
         <v>25</v>
       </c>
-      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="2:7" ht="31.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="3">
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="3:8" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="3">
         <v>26</v>
       </c>
-      <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="5"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
         <v>6</v>
       </c>

</xml_diff>